<commit_message>
Added many characters, color change
</commit_message>
<xml_diff>
--- a/public/data/PlaceHolder.xlsx
+++ b/public/data/PlaceHolder.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\github-tutorial-app\public\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kemok\Desktop\Projects\BEST\Tutorial\github-tutorial-app\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013B6176-8448-4F32-A58D-ABC336E1B356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BF88A5-9C69-447C-81B8-5FF766B1C350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="852" yWindow="840" windowWidth="17280" windowHeight="8880" xr2:uid="{E9C1F2CA-23F5-4C00-976F-C43B9F7B026F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E9C1F2CA-23F5-4C00-976F-C43B9F7B026F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="9">
+  <futureMetadata name="XLRICHVALUE" count="13">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -107,8 +107,36 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="9"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="10"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="11"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="12"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="9">
+  <valueMetadata count="13">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -135,13 +163,25 @@
     </bk>
     <bk>
       <rc t="1" v="8"/>
+    </bk>
+    <bk>
+      <rc t="1" v="9"/>
+    </bk>
+    <bk>
+      <rc t="1" v="10"/>
+    </bk>
+    <bk>
+      <rc t="1" v="11"/>
+    </bk>
+    <bk>
+      <rc t="1" v="12"/>
     </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -213,6 +253,30 @@
   </si>
   <si>
     <t>Pirate</t>
+  </si>
+  <si>
+    <t>Mega Man</t>
+  </si>
+  <si>
+    <t>Robot</t>
+  </si>
+  <si>
+    <t>Natsu</t>
+  </si>
+  <si>
+    <t>Wizard</t>
+  </si>
+  <si>
+    <t>Meliodas</t>
+  </si>
+  <si>
+    <t>Demon</t>
+  </si>
+  <si>
+    <t>Kirby</t>
+  </si>
+  <si>
+    <t>Kirbys</t>
   </si>
 </sst>
 </file>
@@ -322,7 +386,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="9">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="13">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -357,6 +421,22 @@
   </rv>
   <rv s="0">
     <v>8</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>9</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>10</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>11</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>12</v>
     <v>5</v>
   </rv>
 </rvData>
@@ -382,6 +462,10 @@
   <rel r:id="rId7"/>
   <rel r:id="rId8"/>
   <rel r:id="rId9"/>
+  <rel r:id="rId10"/>
+  <rel r:id="rId11"/>
+  <rel r:id="rId12"/>
+  <rel r:id="rId13"/>
 </richValueRels>
 </file>
 
@@ -702,21 +786,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03023D7A-05C0-4155-8EF6-98E874644532}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -730,7 +814,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -744,7 +828,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -758,7 +842,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -772,7 +856,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -786,7 +870,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -800,11 +884,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="e" vm="6">
+      <c r="B7" s="2" t="e" vm="6">
         <v>#VALUE!</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -814,11 +898,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B8" t="e" vm="7">
+      <c r="B8" s="2" t="e" vm="7">
         <v>#VALUE!</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -828,11 +912,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B9" t="e" vm="8">
+      <c r="B9" s="2" t="e" vm="8">
         <v>#VALUE!</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -842,11 +926,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B10" t="e" vm="9">
+      <c r="B10" s="2" t="e" vm="9">
         <v>#VALUE!</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -854,6 +938,62 @@
       </c>
       <c r="D10" s="2" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="2" t="e" vm="10">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="2" t="e" vm="11">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="2" t="e" vm="12">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="2" t="e" vm="13">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>